<commit_message>
Begin integration of binder, colophon, text cleaning
</commit_message>
<xml_diff>
--- a/data/cri_margins.xlsx
+++ b/data/cri_margins.xlsx
@@ -12937,22 +12937,22 @@
         <v>172.0</v>
       </c>
       <c r="D173" t="n">
-        <v>-0.02708</v>
+        <v>-0.02917</v>
       </c>
       <c r="E173" t="n">
-        <v>-0.05208</v>
+        <v>-0.05833</v>
       </c>
       <c r="F173" t="n">
-        <v>-1.0E-5</v>
+        <v>-0.001</v>
       </c>
       <c r="G173" t="n">
-        <v>0.025</v>
+        <v>0.02916</v>
       </c>
       <c r="H173" t="n">
-        <v>-2.03916</v>
+        <v>-1.99385</v>
       </c>
       <c r="I173" t="n">
-        <v>0.04143</v>
+        <v>0.04617</v>
       </c>
     </row>
     <row r="174">
@@ -12966,22 +12966,22 @@
         <v>173.0</v>
       </c>
       <c r="D174" t="n">
-        <v>0.17292</v>
+        <v>0.24375</v>
       </c>
       <c r="E174" t="n">
-        <v>-0.475</v>
+        <v>-0.60625</v>
       </c>
       <c r="F174" t="n">
-        <v>0.85417</v>
+        <v>1.01458</v>
       </c>
       <c r="G174" t="n">
-        <v>0.6479199999999999</v>
+        <v>0.85</v>
       </c>
       <c r="H174" t="n">
-        <v>0.50998</v>
+        <v>0.58951</v>
       </c>
       <c r="I174" t="n">
-        <v>0.61007</v>
+        <v>0.55552</v>
       </c>
     </row>
     <row r="175">

</xml_diff>